<commit_message>
corrigido o calculo de vazao usando formula de potencia
</commit_message>
<xml_diff>
--- a/Documentos/Projeto de ETA, design.xlsx
+++ b/Documentos/Projeto de ETA, design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ProjetoCNPQ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ProjetoCNPQ\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEC283C-92E2-4C4B-B77C-55E904EB5DFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5260828E-0028-4F96-A44F-04C13B57EACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Determinação da Calha Parshall" sheetId="1" r:id="rId1"/>
@@ -3415,12 +3415,12 @@
   <dimension ref="I2:U53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="2" spans="9:21">
+    <row r="2" spans="9:21" ht="12.75">
       <c r="I2" s="5" t="s">
         <v>30</v>
       </c>
@@ -3429,18 +3429,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="9:21">
+    <row r="3" spans="9:21" ht="12.75">
       <c r="T3" s="6"/>
       <c r="U3" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="9:21">
+    <row r="4" spans="9:21" ht="12.75">
       <c r="I4" s="3" t="s">
         <v>38</v>
       </c>
       <c r="J4" s="30">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>43</v>
@@ -3465,7 +3465,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="9:21">
+    <row r="5" spans="9:21" ht="12.75">
       <c r="Q5" s="3" t="s">
         <v>97</v>
       </c>
@@ -3476,12 +3476,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="9:21">
+    <row r="7" spans="9:21" ht="12.75">
       <c r="I7" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="9:21">
+    <row r="9" spans="9:21" ht="12.75">
       <c r="I9" s="5" t="s">
         <v>100</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="11" spans="9:21">
+    <row r="11" spans="9:21" ht="12.75">
       <c r="I11" s="3" t="s">
         <v>101</v>
       </c>
@@ -3502,12 +3502,12 @@
         <v>449</v>
       </c>
     </row>
-    <row r="12" spans="9:21">
+    <row r="12" spans="9:21" ht="12.75">
       <c r="I12" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="9:21">
+    <row r="14" spans="9:21" ht="12.75">
       <c r="I14" s="3" t="s">
         <v>103</v>
       </c>
@@ -3518,8 +3518,12 @@
       <c r="K14" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="9:21">
+      <c r="L14">
+        <f xml:space="preserve"> J16*POWER(J4,J17)</f>
+        <v>4.2540413657195835</v>
+      </c>
+    </row>
+    <row r="16" spans="9:21" ht="12.75">
       <c r="I16" s="3" t="s">
         <v>104</v>
       </c>
@@ -3527,7 +3531,7 @@
         <v>0.60799999999999998</v>
       </c>
     </row>
-    <row r="17" spans="9:10">
+    <row r="17" spans="9:10" ht="12.75">
       <c r="I17" s="3" t="s">
         <v>21</v>
       </c>
@@ -3545,7 +3549,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="53" spans="9:9">
+    <row r="53" spans="9:9" ht="12.75">
       <c r="I53" s="37"/>
     </row>
   </sheetData>
@@ -3575,12 +3579,12 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" ht="12.75">
       <c r="B4" s="5" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" ht="14.25">
       <c r="B6" s="3" t="s">
         <v>267</v>
       </c>
@@ -3591,12 +3595,12 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" ht="12.75">
       <c r="B8" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" ht="12.75">
       <c r="B10" s="3" t="s">
         <v>272</v>
       </c>
@@ -3608,7 +3612,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" ht="12.75">
       <c r="B12" s="3" t="s">
         <v>276</v>
       </c>
@@ -3619,17 +3623,17 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" ht="12.75">
       <c r="B14" s="5" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" ht="12.75">
       <c r="B16" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" ht="12.75">
       <c r="B18" s="3" t="s">
         <v>284</v>
       </c>
@@ -3641,22 +3645,22 @@
         <v>285</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" ht="12.75">
       <c r="B20" s="5" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" ht="12.75">
       <c r="B22" s="5" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" ht="12.75">
       <c r="B24" s="3" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" ht="12.75">
       <c r="B26" s="3" t="s">
         <v>292</v>
       </c>
@@ -3668,12 +3672,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" ht="12.75">
       <c r="B28" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" ht="12.75">
       <c r="B30" s="3" t="s">
         <v>296</v>
       </c>
@@ -3685,7 +3689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" ht="12.75">
       <c r="B32" s="3" t="s">
         <v>299</v>
       </c>
@@ -4055,12 +4059,12 @@
         <v>337</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" ht="12.75">
       <c r="B4" s="5" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" ht="14.25">
       <c r="B6" s="3" t="s">
         <v>75</v>
       </c>
@@ -4072,7 +4076,7 @@
       </c>
       <c r="F6" s="54"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" ht="12.75">
       <c r="B7" s="3" t="s">
         <v>75</v>
       </c>
@@ -4084,7 +4088,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" ht="12.75">
       <c r="B9" s="3" t="s">
         <v>341</v>
       </c>
@@ -4093,15 +4097,15 @@
         <v>2 unidades ou mais</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" ht="12.75">
       <c r="B11" s="5" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" ht="12.75">
       <c r="B14" s="5"/>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" ht="12.75">
       <c r="B16" s="3" t="s">
         <v>75</v>
       </c>
@@ -4109,7 +4113,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" ht="12.75">
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
@@ -4117,7 +4121,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" ht="12.75">
       <c r="B18" s="3" t="s">
         <v>328</v>
       </c>
@@ -4125,7 +4129,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" ht="12.75">
       <c r="B19" s="3" t="s">
         <v>346</v>
       </c>
@@ -4133,10 +4137,10 @@
         <v>347</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" ht="12.75">
       <c r="B20" s="5"/>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" ht="12.75">
       <c r="B22" s="5"/>
     </row>
     <row r="47" spans="2:2" ht="12.75">
@@ -4339,7 +4343,7 @@
     <col min="8" max="8" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:256">
+    <row r="1" spans="2:256" ht="12.75">
       <c r="IV1" s="75">
         <f>0.1</f>
         <v>0.1</v>
@@ -4350,12 +4354,12 @@
         <v>353</v>
       </c>
     </row>
-    <row r="4" spans="2:256">
+    <row r="4" spans="2:256" ht="12.75">
       <c r="B4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:256">
+    <row r="6" spans="2:256" ht="12.75">
       <c r="B6" s="3" t="s">
         <v>226</v>
       </c>
@@ -4369,7 +4373,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="2:256">
+    <row r="7" spans="2:256" ht="12.75">
       <c r="B7" s="3" t="s">
         <v>42</v>
       </c>
@@ -4380,7 +4384,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="2:256">
+    <row r="8" spans="2:256" ht="12.75">
       <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
@@ -4394,13 +4398,13 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="2:256">
+    <row r="9" spans="2:256" ht="14.25">
       <c r="B9" s="3" t="s">
         <v>355</v>
       </c>
       <c r="H9" s="66"/>
     </row>
-    <row r="10" spans="2:256">
+    <row r="10" spans="2:256" ht="14.25">
       <c r="B10" s="4">
         <v>1.2</v>
       </c>
@@ -4412,7 +4416,7 @@
       </c>
       <c r="H10" s="66"/>
     </row>
-    <row r="11" spans="2:256">
+    <row r="11" spans="2:256" ht="14.25">
       <c r="B11" s="4">
         <v>6</v>
       </c>
@@ -4424,7 +4428,7 @@
       </c>
       <c r="H11" s="66"/>
     </row>
-    <row r="12" spans="2:256">
+    <row r="12" spans="2:256" ht="14.25">
       <c r="B12" s="4">
         <v>0.5</v>
       </c>
@@ -4436,7 +4440,7 @@
       </c>
       <c r="H12" s="66"/>
     </row>
-    <row r="13" spans="2:256">
+    <row r="13" spans="2:256" ht="14.25">
       <c r="B13" s="4">
         <v>60</v>
       </c>
@@ -4448,7 +4452,7 @@
       </c>
       <c r="H13" s="66"/>
     </row>
-    <row r="14" spans="2:256">
+    <row r="14" spans="2:256" ht="14.25">
       <c r="B14" s="21">
         <f>RADIANS(B13)</f>
         <v>1.0471975511965976</v>
@@ -4461,20 +4465,20 @@
       </c>
       <c r="H14" s="66"/>
     </row>
-    <row r="15" spans="2:256">
+    <row r="15" spans="2:256" ht="14.25">
       <c r="H15" s="66"/>
     </row>
-    <row r="16" spans="2:256">
+    <row r="16" spans="2:256" ht="12.75">
       <c r="B16" s="5" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" ht="12.75">
       <c r="B18" s="5" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" ht="12.75">
       <c r="B20" s="3" t="s">
         <v>71</v>
       </c>
@@ -4483,23 +4487,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" ht="14.25">
       <c r="B22" s="5" t="s">
         <v>367</v>
       </c>
       <c r="F22" s="54"/>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" ht="12.75">
       <c r="B24" s="91" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" ht="12.75">
       <c r="B25" s="91" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:7" ht="14.25">
       <c r="B27" s="68" t="s">
         <v>371</v>
       </c>
@@ -4511,12 +4515,12 @@
         <v>372</v>
       </c>
     </row>
-    <row r="29" spans="2:7">
+    <row r="29" spans="2:7" ht="12.75">
       <c r="B29" s="5" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="31" spans="2:7">
+    <row r="31" spans="2:7" ht="12.75">
       <c r="B31" s="57" t="s">
         <v>374</v>
       </c>
@@ -4526,7 +4530,7 @@
       <c r="F31" s="72"/>
       <c r="G31" s="72"/>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" ht="12.75">
       <c r="B33" s="3" t="s">
         <v>375</v>
       </c>
@@ -4538,12 +4542,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" ht="12.75">
       <c r="B35" s="5" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" ht="12.75">
       <c r="B37" s="5" t="s">
         <v>377</v>
       </c>
@@ -5364,18 +5368,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" ht="12.75">
       <c r="H3" s="6"/>
       <c r="I3" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" ht="12.75">
       <c r="B4" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" ht="12.75">
       <c r="B6" s="3" t="s">
         <v>40</v>
       </c>
@@ -5386,7 +5390,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" ht="12.75">
       <c r="B7" s="3" t="s">
         <v>44</v>
       </c>
@@ -5394,7 +5398,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" ht="12.75">
       <c r="B8" s="3" t="s">
         <v>47</v>
       </c>
@@ -5402,12 +5406,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:12" ht="12.75">
       <c r="B10" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" ht="12.75">
       <c r="B12" s="3" t="s">
         <v>38</v>
       </c>
@@ -5438,7 +5442,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" ht="12.75">
       <c r="J13" s="3" t="s">
         <v>97</v>
       </c>
@@ -5449,27 +5453,27 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" ht="12.75">
       <c r="B15" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="2:19">
+    <row r="17" spans="2:19" ht="12.75">
       <c r="B17" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:19">
+    <row r="19" spans="2:19" ht="12.75">
       <c r="B19" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="2:19">
+    <row r="20" spans="2:19" ht="12.75">
       <c r="B20" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="2:19">
+    <row r="22" spans="2:19" ht="12.75">
       <c r="B22" s="3" t="s">
         <v>103</v>
       </c>
@@ -5481,7 +5485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:19">
+    <row r="24" spans="2:19" ht="12.75">
       <c r="B24" s="3" t="s">
         <v>104</v>
       </c>
@@ -5490,7 +5494,7 @@
         <v>0.60799999999999998</v>
       </c>
     </row>
-    <row r="25" spans="2:19">
+    <row r="25" spans="2:19" ht="12.75">
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
@@ -5499,24 +5503,24 @@
         <v>0.63900000000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:19">
+    <row r="27" spans="2:19" ht="12.75">
       <c r="B27" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="2:19">
+    <row r="29" spans="2:19" ht="12.75">
       <c r="B29" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="2:19">
+    <row r="31" spans="2:19" ht="12.75">
       <c r="B31" s="5" t="s">
         <v>107</v>
       </c>
       <c r="L31" s="37"/>
       <c r="S31" s="37"/>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" ht="12.75">
       <c r="B33" s="3" t="s">
         <v>108</v>
       </c>
@@ -5528,7 +5532,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" ht="12.75">
       <c r="B35" s="3" t="s">
         <v>109</v>
       </c>
@@ -5539,7 +5543,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="2:4">
+    <row r="36" spans="2:4" ht="12.75">
       <c r="B36" s="3" t="s">
         <v>110</v>
       </c>
@@ -5997,12 +6001,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" ht="12.75">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" ht="12.75">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -6013,7 +6017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" ht="12.75">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -6024,17 +6028,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" ht="12.75">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" ht="12.75">
       <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" ht="12.75">
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
@@ -6046,17 +6050,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" ht="12.75">
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:13" ht="12.75">
       <c r="B17" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:13">
+    <row r="19" spans="2:13" ht="12.75">
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
@@ -6068,17 +6072,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:13">
+    <row r="21" spans="2:13" ht="12.75">
       <c r="B21" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:13" ht="12.75">
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:13" ht="14.25">
       <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
@@ -6106,7 +6110,7 @@
       <c r="L25" s="10"/>
       <c r="M25" s="9"/>
     </row>
-    <row r="27" spans="2:13">
+    <row r="27" spans="2:13" ht="14.25">
       <c r="B27" s="3" t="s">
         <v>18</v>
       </c>
@@ -6125,7 +6129,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="29" spans="2:13">
+    <row r="29" spans="2:13" ht="12.75">
       <c r="B29" s="3" t="s">
         <v>21</v>
       </c>
@@ -6136,17 +6140,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="2:13">
+    <row r="31" spans="2:13" ht="12.75">
       <c r="B31" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" ht="12.75">
       <c r="B33" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" ht="12.75">
       <c r="B35" s="3" t="s">
         <v>25</v>
       </c>
@@ -6158,7 +6162,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" ht="12.75">
       <c r="B37" s="14"/>
     </row>
     <row r="38" spans="2:5" ht="15">
@@ -6354,12 +6358,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:14" ht="12.75">
       <c r="B4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" ht="12.75">
       <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
@@ -6370,7 +6374,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" ht="12.75">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -6399,7 +6403,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" ht="12.75">
       <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
@@ -6410,7 +6414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" ht="12.75">
       <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
@@ -6441,7 +6445,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" ht="12.75">
       <c r="B10" s="3" t="s">
         <v>51</v>
       </c>
@@ -6452,22 +6456,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" ht="12.75">
       <c r="B11" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" ht="12.75">
       <c r="B13" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" ht="12.75">
       <c r="B15" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" ht="12.75">
       <c r="B17" s="3" t="s">
         <v>55</v>
       </c>
@@ -6479,17 +6483,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" ht="12.75">
       <c r="B19" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" ht="12.75">
       <c r="B21" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" ht="12.75">
       <c r="B23" s="3" t="s">
         <v>59</v>
       </c>
@@ -6501,17 +6505,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" ht="12.75">
       <c r="B25" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" ht="12.75">
       <c r="B27" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" ht="12.75">
       <c r="B29" s="3" t="s">
         <v>63</v>
       </c>
@@ -6523,7 +6527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" ht="12.75">
       <c r="B31" s="3" t="s">
         <v>64</v>
       </c>
@@ -6534,7 +6538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
+    <row r="33" spans="2:6" ht="12.75">
       <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
@@ -6546,12 +6550,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:6" ht="12.75">
       <c r="B35" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:6" ht="12.75">
       <c r="B37" s="5" t="s">
         <v>67</v>
       </c>
@@ -7157,12 +7161,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:14" ht="12.75">
       <c r="B4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" ht="12.75">
       <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
@@ -7173,7 +7177,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="2:14" ht="12.75">
       <c r="B7" s="3" t="s">
         <v>35</v>
       </c>
@@ -7202,7 +7206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" ht="12.75">
       <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
@@ -7213,7 +7217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" ht="12.75">
       <c r="B9" s="3" t="s">
         <v>42</v>
       </c>
@@ -7245,7 +7249,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" ht="12.75">
       <c r="B10" s="3" t="s">
         <v>51</v>
       </c>
@@ -7256,22 +7260,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" ht="12.75">
       <c r="B11" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" ht="12.75">
       <c r="B13" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" ht="12.75">
       <c r="B15" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" ht="12.75">
       <c r="B17" s="3" t="s">
         <v>55</v>
       </c>
@@ -7283,17 +7287,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" ht="12.75">
       <c r="B19" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" ht="12.75">
       <c r="B21" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" ht="12.75">
       <c r="B23" s="3" t="s">
         <v>59</v>
       </c>
@@ -7305,17 +7309,17 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" ht="12.75">
       <c r="B25" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" ht="12.75">
       <c r="B27" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" ht="12.75">
       <c r="B29" s="3" t="s">
         <v>63</v>
       </c>
@@ -7327,7 +7331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" ht="12.75">
       <c r="B31" s="3" t="s">
         <v>64</v>
       </c>
@@ -7338,7 +7342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:14">
+    <row r="33" spans="2:14" ht="12.75">
       <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
@@ -7350,7 +7354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:14">
+    <row r="35" spans="2:14" ht="12.75">
       <c r="B35" s="56" t="s">
         <v>184</v>
       </c>
@@ -7374,7 +7378,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="2:14">
+    <row r="37" spans="2:14" ht="12.75">
       <c r="B37" s="5" t="s">
         <v>188</v>
       </c>
@@ -7718,12 +7722,12 @@
         <v>225</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" ht="12.75">
       <c r="B4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" ht="12.75">
       <c r="B6" s="3" t="s">
         <v>226</v>
       </c>
@@ -7737,7 +7741,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" ht="12.75">
       <c r="B7" s="3" t="s">
         <v>42</v>
       </c>
@@ -7748,7 +7752,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" ht="12.75">
       <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
@@ -7762,25 +7766,25 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" ht="14.25">
       <c r="H9" s="66"/>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" ht="12.75">
       <c r="B10" s="5" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" ht="12.75">
       <c r="B12" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" ht="12.75">
       <c r="B14" s="5" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" ht="12.75">
       <c r="B16" s="3" t="s">
         <v>59</v>
       </c>
@@ -7792,7 +7796,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:13" ht="14.25">
       <c r="B18" s="5" t="s">
         <v>234</v>
       </c>
@@ -7800,12 +7804,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="20" spans="2:13">
+    <row r="20" spans="2:13" ht="12.75">
       <c r="B20" s="67" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="22" spans="2:13">
+    <row r="22" spans="2:13" ht="14.25">
       <c r="B22" s="68" t="s">
         <v>77</v>
       </c>
@@ -7839,19 +7843,19 @@
       <c r="L22" s="70"/>
       <c r="M22" s="70"/>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:13" ht="12.75">
       <c r="J23" s="69" t="str">
         <f>IF(C22&gt;I22,"é maior que 2,5 - está ok","não é, corrigir")</f>
         <v>é maior que 2,5 - está ok</v>
       </c>
       <c r="K23" s="70"/>
     </row>
-    <row r="24" spans="2:13">
+    <row r="24" spans="2:13" ht="12.75">
       <c r="B24" s="5" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="26" spans="2:13">
+    <row r="26" spans="2:13" ht="14.25">
       <c r="B26" s="3" t="s">
         <v>254</v>
       </c>
@@ -7862,7 +7866,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="28" spans="2:13">
+    <row r="28" spans="2:13" ht="12.75">
       <c r="B28" s="57" t="s">
         <v>256</v>
       </c>
@@ -7884,7 +7888,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="2:13">
+    <row r="30" spans="2:13" ht="12.75">
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
@@ -7896,7 +7900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:13">
+    <row r="32" spans="2:13" ht="12.75">
       <c r="B32" s="73" t="s">
         <v>8</v>
       </c>
@@ -7907,7 +7911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" ht="12.75">
       <c r="B33" s="73" t="s">
         <v>71</v>
       </c>
@@ -7919,7 +7923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="2:4">
+    <row r="35" spans="2:4" ht="12.75">
       <c r="B35" s="3" t="s">
         <v>282</v>
       </c>
@@ -7931,7 +7935,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="2:4">
+    <row r="37" spans="2:4" ht="12.75">
       <c r="C37" s="3" t="s">
         <v>97</v>
       </c>
@@ -8120,25 +8124,25 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" ht="12.75">
       <c r="B4" s="5" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" ht="12.75">
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" ht="12.75">
       <c r="B6" s="3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" ht="12.75">
       <c r="B8" s="5" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" ht="12.75">
       <c r="B10" s="3" t="s">
         <v>245</v>
       </c>
@@ -8146,7 +8150,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" ht="12.75">
       <c r="B11" s="3" t="s">
         <v>247</v>
       </c>
@@ -8154,7 +8158,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" ht="12.75">
       <c r="B12" s="3" t="s">
         <v>249</v>
       </c>
@@ -8162,7 +8166,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" ht="12.75">
       <c r="B14" s="3" t="s">
         <v>251</v>
       </c>
@@ -8174,7 +8178,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" ht="12.75">
       <c r="B15" s="3" t="s">
         <v>247</v>
       </c>
@@ -8186,7 +8190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" ht="12.75">
       <c r="B16" s="3" t="s">
         <v>249</v>
       </c>
@@ -8198,12 +8202,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" ht="12.75">
       <c r="B18" s="5" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="20" spans="2:9">
+    <row r="20" spans="2:9" ht="12.75">
       <c r="B20" s="3" t="s">
         <v>245</v>
       </c>
@@ -8214,20 +8218,20 @@
         <v>252</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" ht="12.75">
       <c r="B22" s="5" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" ht="12.75">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" ht="12.75">
       <c r="B24" s="5" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" ht="12.75">
       <c r="B26" s="3" t="s">
         <v>264</v>
       </c>
@@ -8239,7 +8243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" ht="14.25">
       <c r="B28" s="3" t="s">
         <v>269</v>
       </c>
@@ -8253,12 +8257,12 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" ht="12.75">
       <c r="B30" s="5" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="32" spans="2:9">
+    <row r="32" spans="2:9" ht="12.75">
       <c r="B32" s="3" t="s">
         <v>275</v>
       </c>
@@ -8270,12 +8274,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:7" ht="12.75">
       <c r="B34" s="5" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="2:7" ht="12.75">
       <c r="B36" s="5" t="s">
         <v>280</v>
       </c>
@@ -8387,12 +8391,12 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:8" ht="12.75">
       <c r="B4" s="5" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" ht="14.25">
       <c r="B6" s="3" t="s">
         <v>267</v>
       </c>
@@ -8403,12 +8407,12 @@
         <v>268</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" ht="12.75">
       <c r="B8" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" ht="12.75">
       <c r="B10" s="3" t="s">
         <v>272</v>
       </c>
@@ -8420,7 +8424,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" ht="12.75">
       <c r="B12" s="3" t="s">
         <v>276</v>
       </c>
@@ -8431,17 +8435,17 @@
         <v>277</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" ht="12.75">
       <c r="B14" s="5" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" ht="12.75">
       <c r="B16" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" ht="12.75">
       <c r="B18" s="3" t="s">
         <v>284</v>
       </c>
@@ -8453,22 +8457,22 @@
         <v>285</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" ht="12.75">
       <c r="B20" s="5" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" ht="12.75">
       <c r="B22" s="5" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" ht="12.75">
       <c r="B24" s="3" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" ht="12.75">
       <c r="B26" s="3" t="s">
         <v>292</v>
       </c>
@@ -8480,12 +8484,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" ht="12.75">
       <c r="B28" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" ht="12.75">
       <c r="B30" s="3" t="s">
         <v>296</v>
       </c>
@@ -8497,7 +8501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" ht="12.75">
       <c r="B32" s="3" t="s">
         <v>299</v>
       </c>

</xml_diff>